<commit_message>
change topoloty.metaData format + add topologyType
</commit_message>
<xml_diff>
--- a/data/topology_FB2024v1.xlsx
+++ b/data/topology_FB2024v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordicrsc-my.sharepoint.com/personal/jlm_nordic-rcc_net/Documents/Dokumenter/topology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="376" documentId="8_{CD18796C-67F4-4BE3-8A85-DF1600E63824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD528EA2-84B7-44C6-A52E-AB0931D78147}"/>
+  <xr:revisionPtr revIDLastSave="377" documentId="8_{CD18796C-67F4-4BE3-8A85-DF1600E63824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6F0634A-5682-45BD-8AFB-C070C74A453F}"/>
   <bookViews>
-    <workbookView xWindow="29370" yWindow="-4800" windowWidth="19125" windowHeight="10035" xr2:uid="{4FBD8BC6-F0E3-4971-A871-8AE8F24F6C5A}"/>
+    <workbookView xWindow="41640" yWindow="150" windowWidth="14340" windowHeight="7245" xr2:uid="{4FBD8BC6-F0E3-4971-A871-8AE8F24F6C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="metaData" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="183">
   <si>
     <t>DK1</t>
   </si>
@@ -583,6 +583,12 @@
   </si>
   <si>
     <t>createdDate</t>
+  </si>
+  <si>
+    <t>topologyType</t>
+  </si>
+  <si>
+    <t>flowBased</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1009,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1024,6 +1030,9 @@
       <c r="D1" t="s">
         <v>166</v>
       </c>
+      <c r="E1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1037,6 +1046,9 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>